<commit_message>
Running project with POM.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Master_Sheet.xlsx
+++ b/src/test/resources/testData/Master_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT-Learn_Automation\WorkSpace\WorkSpace_Photon\SeleniumTraining_B11_MVN\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB2E9DD-E49F-4B5F-80C2-C417018DBF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4C1BCF-A5CB-43BC-86F5-B89D10AF4480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -601,7 +601,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,7 +685,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -740,7 +740,7 @@
         <v>57</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>